<commit_message>
Delete legacy storm dft single run conversion times.
</commit_message>
<xml_diff>
--- a/storm-dft timings.xlsx
+++ b/storm-dft timings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jan.boerman\hobby\FaultTreeHeight\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFDBB554-4E06-43EA-A144-BC1753C61B57}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB2304E2-BCDB-4540-8295-1C5F13D75A9D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13224" windowHeight="5556" xr2:uid="{B4E1E8EA-30D9-4A06-B424-8D7026227DB8}"/>
   </bookViews>
@@ -517,8 +517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0587B059-8986-4E2D-BC0A-85DFA1B2EBAF}">
   <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -580,59 +580,59 @@
         <v>39</v>
       </c>
       <c r="B2" s="3">
-        <f>AVERAGE(B3:B27)</f>
+        <f t="shared" ref="B2:O2" si="0">AVERAGE(B3:B27)</f>
         <v>25.494576560000006</v>
       </c>
       <c r="C2" s="3">
-        <f>AVERAGE(C3:C27)</f>
+        <f t="shared" si="0"/>
         <v>57.855271079999994</v>
       </c>
       <c r="D2" s="3">
-        <f>AVERAGE(D3:D27)</f>
+        <f t="shared" si="0"/>
         <v>48.875466559999992</v>
       </c>
       <c r="E2" s="3">
-        <f>AVERAGE(E3:E27)</f>
+        <f t="shared" si="0"/>
         <v>49.409663839999993</v>
       </c>
       <c r="F2" s="3">
-        <f>AVERAGE(F3:F27)</f>
+        <f t="shared" si="0"/>
         <v>59.033838160000002</v>
       </c>
       <c r="G2" s="3">
-        <f>AVERAGE(G3:G27)</f>
+        <f t="shared" si="0"/>
         <v>61.554788159999987</v>
       </c>
       <c r="H2" s="3">
-        <f>AVERAGE(H3:H27)</f>
+        <f t="shared" si="0"/>
         <v>88.640462239999991</v>
       </c>
       <c r="I2" s="3">
-        <f>AVERAGE(I3:I27)</f>
+        <f t="shared" si="0"/>
         <v>85.565835359999994</v>
       </c>
       <c r="J2" s="3">
-        <f>AVERAGE(J3:J27)</f>
+        <f t="shared" si="0"/>
         <v>61.57743224</v>
       </c>
       <c r="K2" s="3">
-        <f>AVERAGE(K3:K27)</f>
+        <f t="shared" si="0"/>
         <v>100.13385584</v>
       </c>
       <c r="L2" s="3">
-        <f>AVERAGE(L3:L27)</f>
+        <f t="shared" si="0"/>
         <v>120.44976972000001</v>
       </c>
       <c r="M2" s="3">
-        <f>AVERAGE(M3:M27)</f>
+        <f t="shared" si="0"/>
         <v>176.13534224</v>
       </c>
       <c r="N2" s="3">
-        <f>AVERAGE(N3:N27)</f>
+        <f t="shared" si="0"/>
         <v>179.71188160000003</v>
       </c>
       <c r="O2" s="3">
-        <f>AVERAGE(O3:O27)</f>
+        <f t="shared" si="0"/>
         <v>319.47053156000004</v>
       </c>
     </row>

</xml_diff>